<commit_message>
gestion des exceptions, retrait de fonctions innutiles, ajout de la javadoc, explication de l'algorithme utilisé, readme
</commit_message>
<xml_diff>
--- a/Instances-20251127/coutOptimalParInstance.xlsx
+++ b/Instances-20251127/coutOptimalParInstance.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdelobelle/Documents/enseignements/paris/2025-2026/s1/PAA/projet/instance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdelobelle/Documents/enseignements/paris/2025-2026/s1/PAA/projet/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45839DAD-4E0C-DA4B-9825-F5B76646F129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C15C57-01DB-D84A-B9CB-9E5856CC91A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nom fichier</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>instance6</t>
+  </si>
+  <si>
+    <t>instance7</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -451,7 +454,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +483,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3">
         <v>0.95039682539682502</v>
       </c>
     </row>
@@ -505,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="5">
-        <v>23.919019035692099</v>
+        <v>12.504761904761899</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -513,12 +516,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="5">
-        <v>17.8767949002387</v>
+        <v>1.2523809523809499</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>49.884303350970001</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
corretions des intances de test
</commit_message>
<xml_diff>
--- a/Instances-20251127/coutOptimalParInstance.xlsx
+++ b/Instances-20251127/coutOptimalParInstance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdelobelle/Documents/enseignements/paris/2025-2026/s1/PAA/projet/instances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C15C57-01DB-D84A-B9CB-9E5856CC91A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41E61AE-6F5F-DD48-B360-6498701B32D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
+    <workbookView xWindow="32080" yWindow="-1700" windowWidth="28040" windowHeight="16360" xr2:uid="{D15D0B4D-8D42-C74A-86C1-64A36FE8CB57}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -135,8 +135,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +452,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>0.48412698412698402</v>
+        <v>0.69841269841269804</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.95039682539682502</v>
+        <v>1.0595238095238</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -507,24 +505,24 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5">
-        <v>12.504761904761899</v>
+      <c r="B6" s="1">
+        <v>1.5119047619047601</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5">
-        <v>1.2523809523809499</v>
+      <c r="B7" s="1">
+        <v>0.75595238095238004</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
-        <v>49.884303350970001</v>
+      <c r="B8">
+        <v>5.0941798941798897</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>